<commit_message>
Added hospital beds and some other stuff
</commit_message>
<xml_diff>
--- a/Data/Input_Simulador.xlsx
+++ b/Data/Input_Simulador.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B88C04-A71A-4552-8DE4-0FA24CDB1C7C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1FE460-B7FE-49BF-8B34-CC067AD560F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="5520" yWindow="3432" windowWidth="17280" windowHeight="9072" firstSheet="2" activeTab="2" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
-    <sheet name="CapacidadSanitaria" sheetId="22" r:id="rId1"/>
-    <sheet name="CapacidadSanitaria1" sheetId="23" state="hidden" r:id="rId2"/>
-    <sheet name="CapacidadSanitaria2" sheetId="24" state="hidden" r:id="rId3"/>
-    <sheet name="Provincias" sheetId="1" r:id="rId4"/>
-    <sheet name="Diccionario" sheetId="15" r:id="rId5"/>
-    <sheet name="Perfil Etário" sheetId="2" r:id="rId6"/>
-    <sheet name="Capacidad Sanitaria" sheetId="12" r:id="rId7"/>
+    <sheet name="CapacidadSanitaria1" sheetId="23" state="hidden" r:id="rId1"/>
+    <sheet name="CapacidadSanitaria2" sheetId="24" state="hidden" r:id="rId2"/>
+    <sheet name="Provincias" sheetId="1" r:id="rId3"/>
+    <sheet name="Diccionario" sheetId="15" r:id="rId4"/>
+    <sheet name="CapacidadSanitariaCamas" sheetId="27" state="hidden" r:id="rId5"/>
+    <sheet name="Capacidad Sanitaria" sheetId="12" state="hidden" r:id="rId6"/>
+    <sheet name="Perfil Etário" sheetId="2" r:id="rId7"/>
     <sheet name="matrizOD" sheetId="3" r:id="rId8"/>
     <sheet name="TiposdeMovimientos" sheetId="14" r:id="rId9"/>
     <sheet name="Probabilidad de Movimientos" sheetId="25" r:id="rId10"/>
@@ -33,12 +33,13 @@
     <sheet name="TasaGrave" sheetId="21" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Perfil Etário'!$A$1:$F$2725</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">CapacidadSanitariaCamas!$A$1:$D$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Perfil Etário'!$A$1:$F$2725</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Probabilidad de Movimientos'!$A$1:$E$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId19"/>
+    <pivotCache cacheId="0" r:id="rId19"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="171">
   <si>
     <t>id</t>
   </si>
@@ -562,6 +563,12 @@
   </si>
   <si>
     <t>Cantidad de Viajes Diarios</t>
+  </si>
+  <si>
+    <t>Cantidad Terapia Intensiva</t>
+  </si>
+  <si>
+    <t>Cantidad Aislamiento</t>
   </si>
 </sst>
 </file>
@@ -1493,7 +1500,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BD467742-4A03-4442-8CC0-599E387987AD}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BD467742-4A03-4442-8CC0-599E387987AD}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="3">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -1863,255 +1870,1118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66054AC1-CF8C-4A08-A1EB-1F8B507FB863}">
-  <dimension ref="A1:B26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57AA040-B74C-4B71-A1C5-5DD0959FDA89}">
+  <sheetPr>
+    <tabColor theme="9"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B26"/>
+      <selection activeCell="A3" sqref="A3:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="14" style="12"/>
+    <col min="6" max="6" width="21.6640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="27.77734375" style="12" customWidth="1"/>
+    <col min="8" max="8" width="15" style="12" customWidth="1"/>
+    <col min="9" max="9" width="14" style="12"/>
+    <col min="10" max="10" width="29.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="14" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="13">
+        <v>61659</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="13">
+        <v>5273</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="13">
+        <v>3866</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="13">
+        <v>3194</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="13">
+        <v>5640</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1248</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="77" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="76" t="s">
+      <c r="G7" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="13">
+        <v>3945</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A2,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A2,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>4829</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="76" t="s">
+      <c r="G8" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="12" t="str">
+        <f t="shared" ref="I8:I32" si="0">VLOOKUP(J8,$F$8:$G$32,2,FALSE)</f>
+        <v>Centro</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="3">
+        <v>5708369</v>
+      </c>
+      <c r="L8" s="79">
+        <f t="shared" ref="L8:L32" si="1">K8/SUMIF($I$8:$I$32,I8,$K$8:$K$32)</f>
+        <v>0.21742322748106793</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="13">
+        <v>1039</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A3,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A3,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>4049</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="76" t="s">
+      <c r="G9" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Centro</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="3">
+        <v>9916715</v>
+      </c>
+      <c r="L9" s="79">
+        <f t="shared" si="1"/>
+        <v>0.37771282503109355</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="13">
+        <v>75729</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A4,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A4,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>3531</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="76" t="s">
+      <c r="G10" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="I10" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Centro</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="K10">
+        <v>3308876</v>
+      </c>
+      <c r="L10" s="79">
+        <f t="shared" si="1"/>
+        <v>0.12603013211911249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="13">
+        <v>1188</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A5,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A5,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>3382</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="76" t="s">
+      <c r="G11" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Centro</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>3194537</v>
+      </c>
+      <c r="L11" s="79">
+        <f t="shared" si="1"/>
+        <v>0.12167513082067545</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="13">
+        <v>4058</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A6,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A6,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>3182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="76" t="s">
+      <c r="G12" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Centro</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12">
+        <v>2890151</v>
+      </c>
+      <c r="L12" s="79">
+        <f t="shared" si="1"/>
+        <v>0.11008152386918854</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="13">
+        <v>1032</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A7,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A7,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>2914</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="76" t="s">
+      <c r="G13" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Cuyo</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13">
+        <v>1738929</v>
+      </c>
+      <c r="L13" s="79">
+        <f t="shared" si="1"/>
+        <v>0.60965980365277916</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="13">
+        <v>924</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A8,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A8,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>2245</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="76" t="s">
+      <c r="G14" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Noa</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14">
+        <v>1448188</v>
+      </c>
+      <c r="L14" s="79">
+        <f t="shared" si="1"/>
+        <v>0.29486184421099271</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="13">
+        <v>396</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A9,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A9,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>1699</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="76" t="s">
+      <c r="G15" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Centro</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="K15">
+        <v>1235994</v>
+      </c>
+      <c r="L15" s="79">
+        <f t="shared" si="1"/>
+        <v>4.707716067886205E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="13">
+        <v>374</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A10,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A10,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>1226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="76" t="s">
+      <c r="G16" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Noa</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16">
+        <v>1214441</v>
+      </c>
+      <c r="L16" s="79">
+        <f t="shared" si="1"/>
+        <v>0.24726921708054628</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="13">
+        <v>100</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A11,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A11,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="76" t="s">
+      <c r="G17" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Nea</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17">
+        <v>1101593</v>
+      </c>
+      <c r="L17" s="79">
+        <f t="shared" si="1"/>
+        <v>0.29937773279715318</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="13">
+        <v>436</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A12,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A12,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>5785</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="76" t="s">
+      <c r="G18" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="I18" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Nea</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18">
+        <v>1055259</v>
+      </c>
+      <c r="L18" s="79">
+        <f t="shared" si="1"/>
+        <v>0.28678563401709256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="13">
+        <v>420</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A13,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A13,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>2265</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="76" t="s">
+      <c r="G19" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Nea</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19">
+        <v>992595</v>
+      </c>
+      <c r="L19" s="79">
+        <f t="shared" si="1"/>
+        <v>0.26975556370255643</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="13">
+        <v>4218</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A14,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A14,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>1438</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="76" t="s">
+      <c r="G20" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="I20" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Noa</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20">
+        <v>874006</v>
+      </c>
+      <c r="L20" s="79">
+        <f t="shared" si="1"/>
+        <v>0.17795411991500612</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="13">
+        <v>23</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A15,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A15,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="76" t="s">
+      <c r="G21" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I21" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Cuyo</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21">
+        <v>681055</v>
+      </c>
+      <c r="L21" s="79">
+        <f t="shared" si="1"/>
+        <v>0.23877447416009709</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="13">
+        <v>8345</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A16,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A16,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>1738</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="76" t="s">
+      <c r="G22" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I22" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Noa</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22">
+        <v>673307</v>
+      </c>
+      <c r="L22" s="79">
+        <f t="shared" si="1"/>
+        <v>0.13709031129947966</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="13">
+        <v>1111</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A17,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A17,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>1605</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="76" t="s">
+      <c r="G23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Sur</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K23">
+        <v>638645</v>
+      </c>
+      <c r="L23" s="79">
+        <f t="shared" si="1"/>
+        <v>0.26399681870285252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="13">
+        <v>967</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A18,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A18,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="76" t="s">
+      <c r="G24" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Sur</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24">
+        <v>551266</v>
+      </c>
+      <c r="L24" s="79">
+        <f t="shared" si="1"/>
+        <v>0.22787694299500771</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="13">
+        <v>239</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A19,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A19,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>863</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="76" t="s">
+      <c r="G25" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I25" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Nea</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25">
+        <v>530162</v>
+      </c>
+      <c r="L25" s="79">
+        <f t="shared" si="1"/>
+        <v>0.14408106948319779</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="13">
+        <v>721</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A20,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A20,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>401</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="76" t="s">
+      <c r="G26" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Sur</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26">
+        <v>509108</v>
+      </c>
+      <c r="L26" s="79">
+        <f t="shared" si="1"/>
+        <v>0.21045008161994824</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="13">
+        <v>112</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B21" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A21,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A21,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>18709</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="76" t="s">
+      <c r="G27" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Cuyo</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27">
+        <v>432310</v>
+      </c>
+      <c r="L27" s="79">
+        <f t="shared" si="1"/>
+        <v>0.15156572218712377</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="13">
+        <v>613</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A22,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A22,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>18062</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="76" t="s">
+      <c r="G28" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I28" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Noa</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28">
+        <v>367828</v>
+      </c>
+      <c r="L28" s="79">
+        <f t="shared" si="1"/>
+        <v>7.4892515635014936E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="13">
+        <v>243</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B23" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A23,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A23,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>6988</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="76" t="s">
+      <c r="G29" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Noa</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K29">
+        <v>333642</v>
+      </c>
+      <c r="L29" s="79">
+        <f t="shared" si="1"/>
+        <v>6.7931991858960317E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="13">
+        <v>2106</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A24,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A24,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>16341</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="76" t="s">
+      <c r="G30" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I30" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Sur</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K30">
+        <v>318951</v>
+      </c>
+      <c r="L30" s="79">
+        <f t="shared" si="1"/>
+        <v>0.13184484231786597</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="13">
+        <v>142</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A25,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A25,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>56071</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="76" t="s">
+      <c r="G31" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I31" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Sur</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K31">
+        <v>273964</v>
+      </c>
+      <c r="L31" s="79">
+        <f t="shared" si="1"/>
+        <v>0.11324855661456411</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="13">
+        <v>10740</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="64">
-        <f>INT(VLOOKUP(VLOOKUP(A26,CapacidadSanitaria1!$F$7:$G$32,2,FALSE),CapacidadSanitaria2!$A$4:$B$8,2,FALSE)*VLOOKUP(A26,CapacidadSanitaria1!$J$7:$L$32,3,FALSE))</f>
-        <v>32276</v>
+      <c r="G32" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I32" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Sur</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K32">
+        <v>127205</v>
+      </c>
+      <c r="L32" s="79">
+        <f t="shared" si="1"/>
+        <v>5.2582757749761379E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="13">
+        <v>2052</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="13">
+        <v>1783</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="13">
+        <v>1357</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="13">
+        <v>1134</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="13">
+        <v>281</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="13">
+        <v>1073</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="13">
+        <v>630</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="13">
+        <v>2246</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="13">
+        <v>271</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="13">
+        <v>4512</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="13">
+        <v>877</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="13">
+        <v>961</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="13">
+        <v>748</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" s="13">
+        <v>424</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="13">
+        <v>82</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="13">
+        <v>435</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="13">
+        <v>221</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="13">
+        <v>1485</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="13">
+        <v>237</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2123,7 +2993,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E26"/>
+      <selection activeCell="A2" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2620,7 +3490,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3319,7 +4189,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -3605,7 +4475,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -3739,7 +4609,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B5" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -3842,7 +4712,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -3937,1122 +4807,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57AA040-B74C-4B71-A1C5-5DD0959FDA89}">
-  <sheetPr>
-    <tabColor theme="9"/>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:L51"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="33.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="14" style="12"/>
-    <col min="6" max="6" width="21.6640625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="27.77734375" style="12" customWidth="1"/>
-    <col min="8" max="8" width="15" style="12" customWidth="1"/>
-    <col min="9" max="9" width="14" style="12"/>
-    <col min="10" max="10" width="29.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="14" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="13">
-        <v>61659</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="13">
-        <v>5273</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="13">
-        <v>3866</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="13">
-        <v>3194</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="13">
-        <v>5640</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="13">
-        <v>1248</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="13">
-        <v>3945</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I8" s="12" t="str">
-        <f t="shared" ref="I8:I32" si="0">VLOOKUP(J8,$F$8:$G$32,2,FALSE)</f>
-        <v>Centro</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="3">
-        <v>5708369</v>
-      </c>
-      <c r="L8" s="79">
-        <f t="shared" ref="L8:L32" si="1">K8/SUMIF($I$8:$I$32,I8,$K$8:$K$32)</f>
-        <v>0.21742322748106793</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="13">
-        <v>1039</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Centro</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K9" s="3">
-        <v>9916715</v>
-      </c>
-      <c r="L9" s="79">
-        <f t="shared" si="1"/>
-        <v>0.37771282503109355</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="13">
-        <v>75729</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="I10" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Centro</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="K10">
-        <v>3308876</v>
-      </c>
-      <c r="L10" s="79">
-        <f t="shared" si="1"/>
-        <v>0.12603013211911249</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="13">
-        <v>1188</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="I11" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Centro</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K11">
-        <v>3194537</v>
-      </c>
-      <c r="L11" s="79">
-        <f t="shared" si="1"/>
-        <v>0.12167513082067545</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="13">
-        <v>4058</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="I12" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Centro</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="K12">
-        <v>2890151</v>
-      </c>
-      <c r="L12" s="79">
-        <f t="shared" si="1"/>
-        <v>0.11008152386918854</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="13">
-        <v>1032</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I13" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Cuyo</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K13">
-        <v>1738929</v>
-      </c>
-      <c r="L13" s="79">
-        <f t="shared" si="1"/>
-        <v>0.60965980365277916</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="13">
-        <v>924</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I14" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Noa</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="K14">
-        <v>1448188</v>
-      </c>
-      <c r="L14" s="79">
-        <f t="shared" si="1"/>
-        <v>0.29486184421099271</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="13">
-        <v>396</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="I15" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Centro</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="K15">
-        <v>1235994</v>
-      </c>
-      <c r="L15" s="79">
-        <f t="shared" si="1"/>
-        <v>4.707716067886205E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="13">
-        <v>374</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I16" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Noa</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16">
-        <v>1214441</v>
-      </c>
-      <c r="L16" s="79">
-        <f t="shared" si="1"/>
-        <v>0.24726921708054628</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="13">
-        <v>100</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I17" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Nea</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17">
-        <v>1101593</v>
-      </c>
-      <c r="L17" s="79">
-        <f t="shared" si="1"/>
-        <v>0.29937773279715318</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18" s="13">
-        <v>436</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I18" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Nea</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18">
-        <v>1055259</v>
-      </c>
-      <c r="L18" s="79">
-        <f t="shared" si="1"/>
-        <v>0.28678563401709256</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="13">
-        <v>420</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I19" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Nea</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19">
-        <v>992595</v>
-      </c>
-      <c r="L19" s="79">
-        <f t="shared" si="1"/>
-        <v>0.26975556370255643</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="13">
-        <v>4218</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I20" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Noa</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20">
-        <v>874006</v>
-      </c>
-      <c r="L20" s="79">
-        <f t="shared" si="1"/>
-        <v>0.17795411991500612</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="13">
-        <v>23</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="I21" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Cuyo</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K21">
-        <v>681055</v>
-      </c>
-      <c r="L21" s="79">
-        <f t="shared" si="1"/>
-        <v>0.23877447416009709</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="13">
-        <v>8345</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="I22" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Noa</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22">
-        <v>673307</v>
-      </c>
-      <c r="L22" s="79">
-        <f t="shared" si="1"/>
-        <v>0.13709031129947966</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="13">
-        <v>1111</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="I23" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Sur</v>
-      </c>
-      <c r="J23" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="K23">
-        <v>638645</v>
-      </c>
-      <c r="L23" s="79">
-        <f t="shared" si="1"/>
-        <v>0.26399681870285252</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="13">
-        <v>967</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="I24" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Sur</v>
-      </c>
-      <c r="J24" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="K24">
-        <v>551266</v>
-      </c>
-      <c r="L24" s="79">
-        <f t="shared" si="1"/>
-        <v>0.22787694299500771</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="13">
-        <v>239</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="I25" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Nea</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K25">
-        <v>530162</v>
-      </c>
-      <c r="L25" s="79">
-        <f t="shared" si="1"/>
-        <v>0.14408106948319779</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="13">
-        <v>721</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="I26" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Sur</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26">
-        <v>509108</v>
-      </c>
-      <c r="L26" s="79">
-        <f t="shared" si="1"/>
-        <v>0.21045008161994824</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="13">
-        <v>112</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="I27" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Cuyo</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K27">
-        <v>432310</v>
-      </c>
-      <c r="L27" s="79">
-        <f t="shared" si="1"/>
-        <v>0.15156572218712377</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="13">
-        <v>613</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="I28" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Noa</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K28">
-        <v>367828</v>
-      </c>
-      <c r="L28" s="79">
-        <f t="shared" si="1"/>
-        <v>7.4892515635014936E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" s="13">
-        <v>243</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="I29" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Noa</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K29">
-        <v>333642</v>
-      </c>
-      <c r="L29" s="79">
-        <f t="shared" si="1"/>
-        <v>6.7931991858960317E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="13">
-        <v>2106</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="I30" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Sur</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K30">
-        <v>318951</v>
-      </c>
-      <c r="L30" s="79">
-        <f t="shared" si="1"/>
-        <v>0.13184484231786597</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B31" s="13">
-        <v>142</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="I31" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Sur</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K31">
-        <v>273964</v>
-      </c>
-      <c r="L31" s="79">
-        <f t="shared" si="1"/>
-        <v>0.11324855661456411</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="13">
-        <v>10740</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="I32" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Sur</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K32">
-        <v>127205</v>
-      </c>
-      <c r="L32" s="79">
-        <f t="shared" si="1"/>
-        <v>5.2582757749761379E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" s="13">
-        <v>2052</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="13">
-        <v>1783</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" s="13">
-        <v>1357</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="13">
-        <v>1134</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="13">
-        <v>281</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="13">
-        <v>1073</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="13">
-        <v>630</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="13">
-        <v>2246</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="13">
-        <v>271</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42" s="13">
-        <v>4512</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B43" s="13">
-        <v>877</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" s="13">
-        <v>961</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B45" s="13">
-        <v>748</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B46" s="13">
-        <v>424</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B47" s="13">
-        <v>82</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" s="13">
-        <v>435</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B49" s="13">
-        <v>221</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B50" s="13">
-        <v>1485</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B51" s="13">
-        <v>237</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A196945-8CDF-4E80-B63F-133550A997F7}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -5146,15 +4900,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBFD61EF-8890-4F24-B0B0-4C71ECA915F1}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5207,7 +4961,9 @@
       <c r="L1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="1"/>
+      <c r="M1" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2">
@@ -5242,13 +4998,15 @@
       <c r="J2">
         <v>0</v>
       </c>
-      <c r="K2">
-        <v>50</v>
-      </c>
-      <c r="L2">
-        <v>50</v>
-      </c>
-      <c r="M2" s="1"/>
+      <c r="K2" s="64">
+        <v>31049</v>
+      </c>
+      <c r="L2" s="64">
+        <v>1226</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3">
@@ -5283,13 +5041,15 @@
       <c r="J3">
         <v>1</v>
       </c>
-      <c r="K3">
-        <v>50</v>
-      </c>
-      <c r="L3">
-        <v>50</v>
-      </c>
-      <c r="M3" s="1"/>
+      <c r="K3" s="64">
+        <v>53940</v>
+      </c>
+      <c r="L3" s="64">
+        <v>2130</v>
+      </c>
+      <c r="M3" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4">
@@ -5323,11 +5083,14 @@
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4">
-        <v>50</v>
-      </c>
-      <c r="L4">
-        <v>50</v>
+      <c r="K4" s="64">
+        <v>17998</v>
+      </c>
+      <c r="L4" s="64">
+        <v>710</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -5362,11 +5125,14 @@
       <c r="J5">
         <v>0</v>
       </c>
-      <c r="K5">
-        <v>50</v>
-      </c>
-      <c r="L5">
-        <v>50</v>
+      <c r="K5" s="64">
+        <v>17376</v>
+      </c>
+      <c r="L5" s="64">
+        <v>686</v>
+      </c>
+      <c r="M5" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -5401,11 +5167,14 @@
       <c r="J6">
         <v>0</v>
       </c>
-      <c r="K6">
-        <v>50</v>
-      </c>
-      <c r="L6">
-        <v>50</v>
+      <c r="K6" s="64">
+        <v>15720</v>
+      </c>
+      <c r="L6" s="64">
+        <v>620</v>
+      </c>
+      <c r="M6" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -5440,11 +5209,14 @@
       <c r="J7">
         <v>0</v>
       </c>
-      <c r="K7">
-        <v>50</v>
-      </c>
-      <c r="L7">
-        <v>50</v>
+      <c r="K7" s="64">
+        <v>5557</v>
+      </c>
+      <c r="L7" s="64">
+        <v>228</v>
+      </c>
+      <c r="M7">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -5479,11 +5251,14 @@
       <c r="J8">
         <v>0</v>
       </c>
-      <c r="K8">
-        <v>50</v>
-      </c>
-      <c r="L8">
-        <v>50</v>
+      <c r="K8" s="64">
+        <v>4494</v>
+      </c>
+      <c r="L8" s="64">
+        <v>334</v>
+      </c>
+      <c r="M8" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -5518,11 +5293,14 @@
       <c r="J9">
         <v>0</v>
       </c>
-      <c r="K9">
-        <v>50</v>
-      </c>
-      <c r="L9">
-        <v>50</v>
+      <c r="K9" s="64">
+        <v>6723</v>
+      </c>
+      <c r="L9" s="64">
+        <v>265</v>
+      </c>
+      <c r="M9" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -5557,11 +5335,14 @@
       <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10">
-        <v>50</v>
-      </c>
-      <c r="L10">
-        <v>50</v>
+      <c r="K10" s="64">
+        <v>3769</v>
+      </c>
+      <c r="L10" s="64">
+        <v>280</v>
+      </c>
+      <c r="M10">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -5596,11 +5377,14 @@
       <c r="J11">
         <v>0</v>
       </c>
-      <c r="K11">
-        <v>50</v>
-      </c>
-      <c r="L11">
-        <v>50</v>
+      <c r="K11" s="64">
+        <v>3315</v>
+      </c>
+      <c r="L11" s="64">
+        <v>215</v>
+      </c>
+      <c r="M11" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -5635,11 +5419,14 @@
       <c r="J12">
         <v>0</v>
       </c>
-      <c r="K12">
-        <v>50</v>
-      </c>
-      <c r="L12">
-        <v>50</v>
+      <c r="K12" s="64">
+        <v>3176</v>
+      </c>
+      <c r="L12" s="64">
+        <v>206</v>
+      </c>
+      <c r="M12" s="1">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -5674,11 +5461,14 @@
       <c r="J13">
         <v>0</v>
       </c>
-      <c r="K13">
-        <v>50</v>
-      </c>
-      <c r="L13">
-        <v>50</v>
+      <c r="K13" s="64">
+        <v>2987</v>
+      </c>
+      <c r="L13" s="64">
+        <v>194</v>
+      </c>
+      <c r="M13">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -5713,11 +5503,14 @@
       <c r="J14">
         <v>0</v>
       </c>
-      <c r="K14">
-        <v>50</v>
-      </c>
-      <c r="L14">
-        <v>50</v>
+      <c r="K14" s="64">
+        <v>2712</v>
+      </c>
+      <c r="L14" s="64">
+        <v>201</v>
+      </c>
+      <c r="M14" s="1">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -5752,11 +5545,14 @@
       <c r="J15">
         <v>0</v>
       </c>
-      <c r="K15">
-        <v>50</v>
-      </c>
-      <c r="L15">
-        <v>50</v>
+      <c r="K15" s="64">
+        <v>2176</v>
+      </c>
+      <c r="L15" s="64">
+        <v>89</v>
+      </c>
+      <c r="M15" s="1">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -5791,14 +5587,17 @@
       <c r="J16">
         <v>0</v>
       </c>
-      <c r="K16">
-        <v>50</v>
-      </c>
-      <c r="L16">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="K16" s="64">
+        <v>2089</v>
+      </c>
+      <c r="L16" s="64">
+        <v>155</v>
+      </c>
+      <c r="M16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5830,14 +5629,17 @@
       <c r="J17">
         <v>0</v>
       </c>
-      <c r="K17">
-        <v>50</v>
-      </c>
-      <c r="L17">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="K17" s="64">
+        <v>1901</v>
+      </c>
+      <c r="L17" s="64">
+        <v>111</v>
+      </c>
+      <c r="M17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5869,14 +5671,17 @@
       <c r="J18">
         <v>0</v>
       </c>
-      <c r="K18">
-        <v>50</v>
-      </c>
-      <c r="L18">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="K18" s="64">
+        <v>1641</v>
+      </c>
+      <c r="L18" s="64">
+        <v>96</v>
+      </c>
+      <c r="M18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5908,14 +5713,17 @@
       <c r="J19">
         <v>0</v>
       </c>
-      <c r="K19">
-        <v>50</v>
-      </c>
-      <c r="L19">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="K19" s="64">
+        <v>1595</v>
+      </c>
+      <c r="L19" s="64">
+        <v>103</v>
+      </c>
+      <c r="M19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5947,14 +5755,17 @@
       <c r="J20">
         <v>0</v>
       </c>
-      <c r="K20">
-        <v>50</v>
-      </c>
-      <c r="L20">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="K20" s="64">
+        <v>1515</v>
+      </c>
+      <c r="L20" s="64">
+        <v>89</v>
+      </c>
+      <c r="M20" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5986,14 +5797,17 @@
       <c r="J21">
         <v>0</v>
       </c>
-      <c r="K21">
-        <v>50</v>
-      </c>
-      <c r="L21">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="K21" s="64">
+        <v>1381</v>
+      </c>
+      <c r="L21" s="64">
+        <v>56</v>
+      </c>
+      <c r="M21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22">
         <v>21</v>
       </c>
@@ -6025,14 +5839,17 @@
       <c r="J22">
         <v>0</v>
       </c>
-      <c r="K22">
-        <v>50</v>
-      </c>
-      <c r="L22">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="K22" s="64">
+        <v>1141</v>
+      </c>
+      <c r="L22" s="64">
+        <v>84</v>
+      </c>
+      <c r="M22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23">
         <v>22</v>
       </c>
@@ -6064,14 +5881,17 @@
       <c r="J23">
         <v>0</v>
       </c>
-      <c r="K23">
-        <v>50</v>
-      </c>
-      <c r="L23">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="K23" s="64">
+        <v>1035</v>
+      </c>
+      <c r="L23" s="64">
+        <v>77</v>
+      </c>
+      <c r="M23" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6103,14 +5923,17 @@
       <c r="J24">
         <v>0</v>
       </c>
-      <c r="K24">
-        <v>50</v>
-      </c>
-      <c r="L24">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="K24" s="64">
+        <v>949</v>
+      </c>
+      <c r="L24" s="64">
+        <v>55</v>
+      </c>
+      <c r="M24" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6142,14 +5965,17 @@
       <c r="J25">
         <v>0</v>
       </c>
-      <c r="K25">
-        <v>50</v>
-      </c>
-      <c r="L25">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="K25" s="64">
+        <v>815</v>
+      </c>
+      <c r="L25" s="64">
+        <v>48</v>
+      </c>
+      <c r="M25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6181,11 +6007,14 @@
       <c r="J26">
         <v>0</v>
       </c>
-      <c r="K26">
-        <v>50</v>
-      </c>
-      <c r="L26">
-        <v>50</v>
+      <c r="K26" s="64">
+        <v>378</v>
+      </c>
+      <c r="L26" s="64">
+        <v>22</v>
+      </c>
+      <c r="M26" s="1">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -6194,7 +6023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{452B1974-6085-4E5B-A1A7-368CFA643C40}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -6203,7 +6032,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
@@ -6506,14 +6335,998 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28FB71BF-F28D-4EE7-8C32-76A0E766434D}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="78" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="77" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="77" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="64">
+        <v>1226</v>
+      </c>
+      <c r="C2" s="64">
+        <v>31049</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="64">
+        <v>2130</v>
+      </c>
+      <c r="C3" s="64">
+        <v>53940</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="76" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="64">
+        <v>710</v>
+      </c>
+      <c r="C4" s="64">
+        <v>17998</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="64">
+        <v>686</v>
+      </c>
+      <c r="C5" s="64">
+        <v>17376</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="64">
+        <v>620</v>
+      </c>
+      <c r="C6" s="64">
+        <v>15720</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="64">
+        <v>228</v>
+      </c>
+      <c r="C7" s="64">
+        <v>5557</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="64">
+        <v>334</v>
+      </c>
+      <c r="C8" s="64">
+        <v>4494</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="76" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="64">
+        <v>265</v>
+      </c>
+      <c r="C9" s="64">
+        <v>6723</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="64">
+        <v>280</v>
+      </c>
+      <c r="C10" s="64">
+        <v>3769</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="64">
+        <v>215</v>
+      </c>
+      <c r="C11" s="64">
+        <v>3315</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="64">
+        <v>206</v>
+      </c>
+      <c r="C12" s="64">
+        <v>3176</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="76" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="64">
+        <v>194</v>
+      </c>
+      <c r="C13" s="64">
+        <v>2987</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="76" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="64">
+        <v>201</v>
+      </c>
+      <c r="C14" s="64">
+        <v>2712</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="76" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="64">
+        <v>89</v>
+      </c>
+      <c r="C15" s="64">
+        <v>2176</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="64">
+        <v>155</v>
+      </c>
+      <c r="C16" s="64">
+        <v>2089</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="64">
+        <v>111</v>
+      </c>
+      <c r="C17" s="64">
+        <v>1901</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="64">
+        <v>96</v>
+      </c>
+      <c r="C18" s="64">
+        <v>1641</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="64">
+        <v>103</v>
+      </c>
+      <c r="C19" s="64">
+        <v>1595</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="64">
+        <v>89</v>
+      </c>
+      <c r="C20" s="64">
+        <v>1515</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="64">
+        <v>56</v>
+      </c>
+      <c r="C21" s="64">
+        <v>1381</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="64">
+        <v>84</v>
+      </c>
+      <c r="C22" s="64">
+        <v>1141</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="64">
+        <v>77</v>
+      </c>
+      <c r="C23" s="64">
+        <v>1035</v>
+      </c>
+      <c r="D23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="64">
+        <v>55</v>
+      </c>
+      <c r="C24" s="64">
+        <v>949</v>
+      </c>
+      <c r="D24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="76" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="64">
+        <v>48</v>
+      </c>
+      <c r="C25" s="64">
+        <v>815</v>
+      </c>
+      <c r="D25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="64">
+        <v>22</v>
+      </c>
+      <c r="C26" s="64">
+        <v>378</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D26" xr:uid="{B82AAB80-C868-4E92-A92F-EEBB6005528C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D26">
+      <sortCondition ref="D1:D26"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D26">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F02907-B371-410B-8844-7370871E290C}">
+  <sheetPr>
+    <tabColor theme="9"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:E51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="33.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="14" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="13">
+        <v>61659</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="13">
+        <v>5273</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="13">
+        <v>3866</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="13">
+        <v>3194</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="13">
+        <v>5640</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1248</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="13">
+        <v>3945</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="13">
+        <v>1039</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="13">
+        <v>75729</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="13">
+        <v>1188</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="13">
+        <v>4058</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="13">
+        <v>1032</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="13">
+        <v>924</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="13">
+        <v>396</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="13">
+        <v>374</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="13">
+        <v>100</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="13">
+        <v>436</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="13">
+        <v>420</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="13">
+        <v>4218</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="13">
+        <v>23</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="13">
+        <v>8345</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="13">
+        <v>1111</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="13">
+        <v>967</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="13">
+        <v>239</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="13">
+        <v>721</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="13">
+        <v>112</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="13">
+        <v>613</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="13">
+        <v>243</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="13">
+        <v>2106</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="13">
+        <v>142</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="13">
+        <v>10740</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="13">
+        <v>2052</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="13">
+        <v>1783</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="13">
+        <v>1357</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="13">
+        <v>1134</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="13">
+        <v>281</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="13">
+        <v>1073</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="13">
+        <v>630</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="13">
+        <v>2246</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="13">
+        <v>271</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="13">
+        <v>4512</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="13">
+        <v>877</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="13">
+        <v>961</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="13">
+        <v>748</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" s="13">
+        <v>424</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="13">
+        <v>82</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="13">
+        <v>435</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="13">
+        <v>221</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="13">
+        <v>1485</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="13">
+        <v>237</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8EFC4FE-610E-497E-93FF-F825D6C88A88}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:F2725"/>
   <sheetViews>
-    <sheetView topLeftCell="A2489" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2720" sqref="H2720"/>
     </sheetView>
   </sheetViews>
@@ -66474,597 +67287,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F2725" xr:uid="{28B7A5E2-2FCF-4944-A8EE-83389D036FB8}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F02907-B371-410B-8844-7370871E290C}">
-  <sheetPr>
-    <tabColor theme="9"/>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:E51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="33.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="14" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="13">
-        <v>61659</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="13">
-        <v>5273</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="13">
-        <v>3866</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="13">
-        <v>3194</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="13">
-        <v>5640</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="13">
-        <v>1248</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="13">
-        <v>3945</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="13">
-        <v>1039</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="13">
-        <v>75729</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="13">
-        <v>1188</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="13">
-        <v>4058</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="13">
-        <v>1032</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="13">
-        <v>924</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="13">
-        <v>396</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="13">
-        <v>374</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="13">
-        <v>100</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18" s="13">
-        <v>436</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="13">
-        <v>420</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="13">
-        <v>4218</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="13">
-        <v>23</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="13">
-        <v>8345</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="13">
-        <v>1111</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="13">
-        <v>967</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="13">
-        <v>239</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="13">
-        <v>721</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="13">
-        <v>112</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="13">
-        <v>613</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" s="13">
-        <v>243</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="13">
-        <v>2106</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B31" s="13">
-        <v>142</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="13">
-        <v>10740</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" s="13">
-        <v>2052</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="13">
-        <v>1783</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" s="13">
-        <v>1357</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="13">
-        <v>1134</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="13">
-        <v>281</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="13">
-        <v>1073</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="13">
-        <v>630</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="13">
-        <v>2246</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="13">
-        <v>271</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42" s="13">
-        <v>4512</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B43" s="13">
-        <v>877</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" s="13">
-        <v>961</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B45" s="13">
-        <v>748</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B46" s="13">
-        <v>424</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B47" s="13">
-        <v>82</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" s="13">
-        <v>435</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B49" s="13">
-        <v>221</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B50" s="13">
-        <v>1485</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B51" s="13">
-        <v>237</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>